<commit_message>
add missing old authors, fix duplicated pubs
</commit_message>
<xml_diff>
--- a/data/Research metrics new 1.xlsx
+++ b/data/Research metrics new 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29728"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qinzen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEBCBFD6-9B8A-49B1-8AAB-31964C5425DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF3C73B9-AAFF-41E1-BD25-4ADA06165AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4266" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4335" uniqueCount="905">
   <si>
     <t>Id</t>
   </si>
@@ -419,6 +419,9 @@
     <t>Texas hornshell annual survey on the Black River</t>
   </si>
   <si>
+    <t>Chicago River board of trustees boat cruise - tabling and also gave a talk</t>
+  </si>
+  <si>
     <t>Presented color changing corals at ACS division meeting</t>
   </si>
   <si>
@@ -443,9 +446,6 @@
     <t>Kayaking event with NFWF personnel and their donors.</t>
   </si>
   <si>
-    <t>Chicago River board of trustees boat cruise - tabling and also gave a talk</t>
-  </si>
-  <si>
     <t>Trustee Event tabling event</t>
   </si>
   <si>
@@ -536,6 +536,9 @@
     <t>Marine ACCA;Marine invertebrates;</t>
   </si>
   <si>
+    <t>Marine Ecology ACCA Course field component CRII (18 days X 8 hours X 18 students)</t>
+  </si>
+  <si>
     <t>ACCA Marine Ecology course Classroom portion only</t>
   </si>
   <si>
@@ -566,9 +569,6 @@
     <t xml:space="preserve">Lunch and Learn on Coral Spawning </t>
   </si>
   <si>
-    <t>Marine Ecology ACCA Course field component CRII (18 days X 8 hours X 18 students)</t>
-  </si>
-  <si>
     <t>Fieldwork in Hawaii with the Coral Resilience Lab studying the impact of translocation on coral microbial communities and gene expression</t>
   </si>
   <si>
@@ -1055,6 +1055,12 @@
     <t>https://www.outdoornews.com/2024/11/27/project-on-understudied-yet-essential-sucker-took-birding-approach-to-studying-fish/</t>
   </si>
   <si>
+    <t>SCTLD Heritability Project Final Presentation to Funders</t>
+  </si>
+  <si>
+    <t>Microbial ecology</t>
+  </si>
+  <si>
     <t>Invited seminar at University of South Florida</t>
   </si>
   <si>
@@ -1136,12 +1142,6 @@
     <t>3rd Q field days</t>
   </si>
   <si>
-    <t>SCTLD Heritability Project Final Presentation to Funders</t>
-  </si>
-  <si>
-    <t>Microbial ecology</t>
-  </si>
-  <si>
     <t>Coral Spawning Research Cruise</t>
   </si>
   <si>
@@ -1235,12 +1235,12 @@
     <t>WBEZ Curious City</t>
   </si>
   <si>
+    <t>Aquatic Science Connection - St Laurence HS Connection</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coral Spawn Research Cruise </t>
   </si>
   <si>
-    <t>Aquatic Science Connection - St Laurence HS Connection</t>
-  </si>
-  <si>
     <t>Port Everglades Coral DRM survey trip</t>
   </si>
   <si>
@@ -1253,33 +1253,33 @@
     <t>https://www.nature.com/articles/s41559-024-02386-9#citeas</t>
   </si>
   <si>
+    <t>Hours for Paula Otu and Noah Kaplan mentoring</t>
+  </si>
+  <si>
     <t>ASM summer programs data analysis workshop</t>
   </si>
   <si>
     <t>Learning</t>
   </si>
   <si>
-    <t>Hours for Paula Otu and Noah Kaplan mentoring</t>
-  </si>
-  <si>
     <t>Freshwater Ecology ACCA Course (18 students X 7 hours X 7 classes)</t>
   </si>
   <si>
+    <t>mussel surveys on St. Croix River with MNDNR+ sample collection at Genoa National Hatchery</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lecture on shark ecology, conservation and research at the Day Star Academy to middle school children - around 25 students in attendance </t>
   </si>
   <si>
     <t>Sustainable fisheries;Habitat and species loss;Climate change</t>
   </si>
   <si>
+    <t>After school matters workshop</t>
+  </si>
+  <si>
     <t>Shark Lecture to Marine ACCA class</t>
   </si>
   <si>
-    <t>After school matters workshop</t>
-  </si>
-  <si>
-    <t>mussel surveys on St. Croix River with MNDNR+ sample collection at Genoa National Hatchery</t>
-  </si>
-  <si>
     <t xml:space="preserve">After School Matters field excursion </t>
   </si>
   <si>
@@ -1328,6 +1328,9 @@
     <t>Gave a career day presentation to 48 junior and seniors at Lockport HS about working as a scientist, and how to pursue a research career</t>
   </si>
   <si>
+    <t>Mentorship calls or letters of rec for various ACCA students (Abigail, Gigi, Isabella, Trista, Aina, Ashleigh, Austin, Alyson, Nikki, Carson))</t>
+  </si>
+  <si>
     <t>Presentation to ASM group on career path and using acoustics in the field</t>
   </si>
   <si>
@@ -1337,9 +1340,6 @@
     <t>Research cruise on the CRii alongside team coral to survey corals in PtEv and to relocate and replace tags on queen conch</t>
   </si>
   <si>
-    <t>Mentorship calls or letters of rec for various ACCA students (Abigail, Gigi, Isabella, Trista, Aina, Ashleigh, Austin, Alyson, Nikki, Carson))</t>
-  </si>
-  <si>
     <t>Career chat with guest engagement staff (Noah, Rosemary, Caslyn, Sarah, Nasr)</t>
   </si>
   <si>
@@ -1394,15 +1394,15 @@
     <t>Q3: Mentored graduate students (Gabe Inoshita, Miami University; Kevin Soto, University of Costa Rica). Engagement includes online meetings, manuscript/thesis proposal reviews, data analysis assistance, and graduate committee duties.</t>
   </si>
   <si>
+    <t>Boman, E. M., de Graaf, M., Kough, A. S., Izioka-Kuramae, A., Zuur, A. F., Smaal, A., &amp; Nagelkerke, L. (2021). Spatial dependency in abundance of Queen conch, Aliger gigas, in the Caribbean, indicates the importance of surveying deep-water distributions. Diversity and Distributions, 27, 2157–2169. https://doi.org/10.1111/ddi.13392</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1111/ddi.13392</t>
+  </si>
+  <si>
     <t>Q4: Mentored graduate students (Gabby Sanfilippo, Central Michigan University; Gabe Inoshita, Miami University; Kevin Soto, University of Costa Rica). Engagement includes online meetings, manuscript/thesis proposal reviews, data analysis assistance, graduate committee duties, and attending Gabe's thesis defense at Miami University.</t>
   </si>
   <si>
-    <t>Boman, E. M., de Graaf, M., Kough, A. S., Izioka-Kuramae, A., Zuur, A. F., Smaal, A., &amp; Nagelkerke, L. (2021). Spatial dependency in abundance of Queen conch, Aliger gigas, in the Caribbean, indicates the importance of surveying deep-water distributions. Diversity and Distributions, 27, 2157–2169. https://doi.org/10.1111/ddi.13392</t>
-  </si>
-  <si>
-    <t>https://onlinelibrary.wiley.com/doi/full/10.1111/ddi.13392</t>
-  </si>
-  <si>
     <t>https://news.wttw.com/2024/12/03/unglamorous-sucker-fish-plays-key-great-lakes-role-shedd-scientist-and-her-band</t>
   </si>
   <si>
@@ -2697,6 +2697,60 @@
   </si>
   <si>
     <t>Met with a undergrad aspiring marine biologist from San Diego to discuss grad school and career path options</t>
+  </si>
+  <si>
+    <t>Field research: The number of days working in the field.  When multiple team members are in the field together, all should enter independently.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American Samoa Field work </t>
+  </si>
+  <si>
+    <t>Presentation: Represents traditional scientific conference presentations, seminars, panel discussions, traditional class lectures, Lunch &amp; Learns, tours, tabling events. If two team members are at an event (e.g., tabling), both team members can enter their participation.</t>
+  </si>
+  <si>
+    <t>Class lecture</t>
+  </si>
+  <si>
+    <t>DePaul Conservation Biology class</t>
+  </si>
+  <si>
+    <t>Conference</t>
+  </si>
+  <si>
+    <t>National PARC updates for Midwest Fish and Wildlife Conference MWPARC symposium</t>
+  </si>
+  <si>
+    <t>Poster of wildlife road mortality at Midwest Fish and Wildlife Conference</t>
+  </si>
+  <si>
+    <t>Media Opportunity: Represents output typically sourced through Shedd’s External Affairs and Marketing team including blogs, internet and print articles; social media placement; podcast, radio, print and television interviews.</t>
+  </si>
+  <si>
+    <t>Social media</t>
+  </si>
+  <si>
+    <t>Instagram posts for wetlands week</t>
+  </si>
+  <si>
+    <t>Community Engagement: Number of people benefiting from training or experiences provided by team members including field assistants, ACCA students on the boat or locally who gain hands-on field experience, interns, volunteers, participants in conservation action planning, etc. If two team members are involved, only one team member should enter the number of people so not to overinflate counts.</t>
+  </si>
+  <si>
+    <t>Volunteers</t>
+  </si>
+  <si>
+    <t>Jackie Aparicio start date</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>Exchanged information for the Lampsilis higginsii recovery efforts</t>
+  </si>
+  <si>
+    <t>Teen ESA panel</t>
+  </si>
+  <si>
+    <t>After-School-Matters internship program</t>
   </si>
 </sst>
 </file>
@@ -2803,8 +2857,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:R603" totalsRowShown="0">
-  <autoFilter ref="A1:R603" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:R613" totalsRowShown="0">
+  <autoFilter ref="A1:R613" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R613">
+    <sortCondition ref="B1:B613"/>
+  </sortState>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="14">
       <extLst>
@@ -2936,7 +2993,7 @@
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{839C7E11-91E4-4DBD-9C5D-0DEA604FA9AC}">
-      <xlmsforms:msForm id="WmKV9QsF-ESGzEsfiGZoTb83Sl3n5wlHr3isCMIkazlUREdPWjQwWjdHU1IxNFdNOVVTSVpHNktFSi4u" isFormConnected="1" maxResponseId="604" latestEventMarker="617">
+      <xlmsforms:msForm id="WmKV9QsF-ESGzEsfiGZoTb83Sl3n5wlHr3isCMIkazlUREdPWjQwWjdHU1IxNFdNOVVTSVpHNktFSi4u" isFormConnected="1" maxResponseId="614" latestEventMarker="627">
         <xlmsforms:syncedQuestionId>id</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>startDate</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>submitDate</xlmsforms:syncedQuestionId>
@@ -3258,9 +3315,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R603"/>
+  <dimension ref="A1:R613"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A580" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A604" sqref="A604"/>
     </sheetView>
   </sheetViews>
@@ -5531,25 +5588,25 @@
     </row>
     <row r="62" spans="1:18">
       <c r="A62">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B62" s="4">
-        <v>45467.434687499997</v>
+        <v>45467.420578703706</v>
       </c>
       <c r="C62" s="4">
-        <v>45467.435844907406</v>
+        <v>45467.513425925928</v>
       </c>
       <c r="D62" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="E62" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="F62" t="s">
         <v>20</v>
       </c>
       <c r="G62" s="1">
-        <v>45441</v>
+        <v>45456</v>
       </c>
       <c r="H62" t="s">
         <v>28</v>
@@ -5558,97 +5615,91 @@
         <v>127</v>
       </c>
       <c r="Q62" t="s">
-        <v>24</v>
-      </c>
-      <c r="R62" t="s">
-        <v>25</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:18">
       <c r="A63">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" s="4">
-        <v>45467.437962962962</v>
+        <v>45467.434687499997</v>
       </c>
       <c r="C63" s="4">
-        <v>45467.438935185186</v>
+        <v>45467.435844907406</v>
       </c>
       <c r="D63" t="s">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="E63" t="s">
-        <v>115</v>
+        <v>19</v>
       </c>
       <c r="F63" t="s">
         <v>20</v>
       </c>
       <c r="G63" s="1">
-        <v>45452</v>
+        <v>45441</v>
       </c>
       <c r="H63" t="s">
-        <v>46</v>
-      </c>
-      <c r="O63">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="P63" t="s">
         <v>128</v>
       </c>
       <c r="Q63" t="s">
-        <v>117</v>
+        <v>24</v>
       </c>
       <c r="R63" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:18">
       <c r="A64">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" s="4">
-        <v>45467.50540509259</v>
+        <v>45467.437962962962</v>
       </c>
       <c r="C64" s="4">
-        <v>45467.506006944444</v>
+        <v>45467.438935185186</v>
       </c>
       <c r="D64" t="s">
-        <v>58</v>
+        <v>114</v>
       </c>
       <c r="E64" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
       <c r="F64" t="s">
         <v>20</v>
       </c>
       <c r="G64" s="1">
-        <v>45464</v>
+        <v>45452</v>
       </c>
       <c r="H64" t="s">
-        <v>21</v>
-      </c>
-      <c r="M64" t="s">
+        <v>46</v>
+      </c>
+      <c r="O64">
+        <v>10</v>
+      </c>
+      <c r="P64" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>117</v>
+      </c>
+      <c r="R64" t="s">
         <v>130</v>
-      </c>
-      <c r="P64" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q64" t="s">
-        <v>62</v>
-      </c>
-      <c r="R64" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:18">
       <c r="A65">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" s="4">
-        <v>45467.506064814814</v>
+        <v>45467.50540509259</v>
       </c>
       <c r="C65" s="4">
-        <v>45467.506886574076</v>
+        <v>45467.506006944444</v>
       </c>
       <c r="D65" t="s">
         <v>58</v>
@@ -5660,13 +5711,13 @@
         <v>20</v>
       </c>
       <c r="G65" s="1">
-        <v>45433</v>
+        <v>45464</v>
       </c>
       <c r="H65" t="s">
-        <v>46</v>
-      </c>
-      <c r="O65">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="M65" t="s">
+        <v>131</v>
       </c>
       <c r="P65" t="s">
         <v>132</v>
@@ -5674,16 +5725,19 @@
       <c r="Q65" t="s">
         <v>62</v>
       </c>
+      <c r="R65" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="66" spans="1:18">
       <c r="A66">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" s="4">
-        <v>45467.506898148145</v>
+        <v>45467.506064814814</v>
       </c>
       <c r="C66" s="4">
-        <v>45467.507824074077</v>
+        <v>45467.506886574076</v>
       </c>
       <c r="D66" t="s">
         <v>58</v>
@@ -5695,13 +5749,13 @@
         <v>20</v>
       </c>
       <c r="G66" s="1">
-        <v>45420</v>
+        <v>45433</v>
       </c>
       <c r="H66" t="s">
         <v>46</v>
       </c>
       <c r="O66">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P66" t="s">
         <v>133</v>
@@ -5712,13 +5766,13 @@
     </row>
     <row r="67" spans="1:18">
       <c r="A67">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" s="4">
-        <v>45467.507847222223</v>
+        <v>45467.506898148145</v>
       </c>
       <c r="C67" s="4">
-        <v>45467.510185185187</v>
+        <v>45467.507824074077</v>
       </c>
       <c r="D67" t="s">
         <v>58</v>
@@ -5730,16 +5784,13 @@
         <v>20</v>
       </c>
       <c r="G67" s="1">
-        <v>45447</v>
+        <v>45420</v>
       </c>
       <c r="H67" t="s">
-        <v>48</v>
-      </c>
-      <c r="N67">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="O67">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="P67" t="s">
         <v>134</v>
@@ -5747,40 +5798,46 @@
       <c r="Q67" t="s">
         <v>62</v>
       </c>
-      <c r="R67" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="68" spans="1:18">
       <c r="A68">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68" s="4">
-        <v>45467.420578703706</v>
+        <v>45467.507847222223</v>
       </c>
       <c r="C68" s="4">
-        <v>45467.513425925928</v>
+        <v>45467.510185185187</v>
       </c>
       <c r="D68" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="E68" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="F68" t="s">
         <v>20</v>
       </c>
       <c r="G68" s="1">
-        <v>45456</v>
+        <v>45447</v>
       </c>
       <c r="H68" t="s">
-        <v>28</v>
+        <v>48</v>
+      </c>
+      <c r="N68">
+        <v>12</v>
+      </c>
+      <c r="O68">
+        <v>12</v>
       </c>
       <c r="P68" t="s">
         <v>135</v>
       </c>
       <c r="Q68" t="s">
-        <v>123</v>
+        <v>62</v>
+      </c>
+      <c r="R68" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="69" spans="1:18">
@@ -6385,7 +6442,7 @@
         <v>117</v>
       </c>
       <c r="R84" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:18">
@@ -6533,31 +6590,31 @@
     </row>
     <row r="89" spans="1:18">
       <c r="A89">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B89" s="4">
-        <v>45476.423692129632</v>
+        <v>45476.407210648147</v>
       </c>
       <c r="C89" s="4">
-        <v>45476.442303240743</v>
+        <v>45476.451041666667</v>
       </c>
       <c r="D89" t="s">
-        <v>26</v>
+        <v>160</v>
       </c>
       <c r="E89" t="s">
-        <v>27</v>
+        <v>161</v>
       </c>
       <c r="F89" t="s">
         <v>20</v>
       </c>
       <c r="G89" s="1">
-        <v>45367</v>
+        <v>45418</v>
       </c>
       <c r="H89" t="s">
         <v>48</v>
       </c>
       <c r="N89">
-        <v>864</v>
+        <v>2592</v>
       </c>
       <c r="O89">
         <v>18</v>
@@ -6566,21 +6623,18 @@
         <v>166</v>
       </c>
       <c r="Q89" t="s">
-        <v>167</v>
-      </c>
-      <c r="R89" t="s">
-        <v>31</v>
+        <v>163</v>
       </c>
     </row>
     <row r="90" spans="1:18">
       <c r="A90">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B90" s="4">
-        <v>45476.442361111112</v>
+        <v>45476.423692129632</v>
       </c>
       <c r="C90" s="4">
-        <v>45476.443229166667</v>
+        <v>45476.442303240743</v>
       </c>
       <c r="D90" t="s">
         <v>26</v>
@@ -6595,13 +6649,19 @@
         <v>45367</v>
       </c>
       <c r="H90" t="s">
-        <v>28</v>
+        <v>48</v>
+      </c>
+      <c r="N90">
+        <v>864</v>
+      </c>
+      <c r="O90">
+        <v>18</v>
       </c>
       <c r="P90" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q90" t="s">
         <v>168</v>
-      </c>
-      <c r="Q90" t="s">
-        <v>169</v>
       </c>
       <c r="R90" t="s">
         <v>31</v>
@@ -6609,13 +6669,13 @@
     </row>
     <row r="91" spans="1:18">
       <c r="A91">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91" s="4">
-        <v>45476.443252314813</v>
+        <v>45476.442361111112</v>
       </c>
       <c r="C91" s="4">
-        <v>45476.443437499998</v>
+        <v>45476.443229166667</v>
       </c>
       <c r="D91" t="s">
         <v>26</v>
@@ -6627,16 +6687,16 @@
         <v>20</v>
       </c>
       <c r="G91" s="1">
-        <v>45493</v>
+        <v>45367</v>
       </c>
       <c r="H91" t="s">
         <v>28</v>
       </c>
       <c r="P91" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q91" t="s">
         <v>170</v>
-      </c>
-      <c r="Q91" t="s">
-        <v>169</v>
       </c>
       <c r="R91" t="s">
         <v>31</v>
@@ -6644,13 +6704,13 @@
     </row>
     <row r="92" spans="1:18">
       <c r="A92">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B92" s="4">
-        <v>45476.443460648145</v>
+        <v>45476.443252314813</v>
       </c>
       <c r="C92" s="4">
-        <v>45476.444247685184</v>
+        <v>45476.443437499998</v>
       </c>
       <c r="D92" t="s">
         <v>26</v>
@@ -6662,7 +6722,7 @@
         <v>20</v>
       </c>
       <c r="G92" s="1">
-        <v>45395</v>
+        <v>45493</v>
       </c>
       <c r="H92" t="s">
         <v>28</v>
@@ -6671,7 +6731,7 @@
         <v>171</v>
       </c>
       <c r="Q92" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="R92" t="s">
         <v>31</v>
@@ -6679,13 +6739,13 @@
     </row>
     <row r="93" spans="1:18">
       <c r="A93">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93" s="4">
-        <v>45476.44427083333</v>
+        <v>45476.443460648145</v>
       </c>
       <c r="C93" s="4">
-        <v>45476.447465277779</v>
+        <v>45476.444247685184</v>
       </c>
       <c r="D93" t="s">
         <v>26</v>
@@ -6697,22 +6757,16 @@
         <v>20</v>
       </c>
       <c r="G93" s="1">
-        <v>45418</v>
+        <v>45395</v>
       </c>
       <c r="H93" t="s">
-        <v>48</v>
-      </c>
-      <c r="N93">
-        <v>810</v>
-      </c>
-      <c r="O93">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="P93" t="s">
         <v>172</v>
       </c>
       <c r="Q93" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="R93" t="s">
         <v>31</v>
@@ -6720,13 +6774,13 @@
     </row>
     <row r="94" spans="1:18">
       <c r="A94">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B94" s="4">
-        <v>45476.447476851848</v>
+        <v>45476.44427083333</v>
       </c>
       <c r="C94" s="4">
-        <v>45476.448576388888</v>
+        <v>45476.447465277779</v>
       </c>
       <c r="D94" t="s">
         <v>26</v>
@@ -6738,19 +6792,22 @@
         <v>20</v>
       </c>
       <c r="G94" s="1">
-        <v>45416</v>
+        <v>45418</v>
       </c>
       <c r="H94" t="s">
-        <v>21</v>
-      </c>
-      <c r="M94" t="s">
+        <v>48</v>
+      </c>
+      <c r="N94">
+        <v>810</v>
+      </c>
+      <c r="O94">
+        <v>9</v>
+      </c>
+      <c r="P94" t="s">
         <v>173</v>
       </c>
-      <c r="P94" t="s">
-        <v>174</v>
-      </c>
       <c r="Q94" t="s">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="R94" t="s">
         <v>31</v>
@@ -6758,13 +6815,13 @@
     </row>
     <row r="95" spans="1:18">
       <c r="A95">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95" s="4">
-        <v>45476.448657407411</v>
+        <v>45476.447476851848</v>
       </c>
       <c r="C95" s="4">
-        <v>45476.450624999998</v>
+        <v>45476.448576388888</v>
       </c>
       <c r="D95" t="s">
         <v>26</v>
@@ -6776,10 +6833,13 @@
         <v>20</v>
       </c>
       <c r="G95" s="1">
-        <v>45405</v>
+        <v>45416</v>
       </c>
       <c r="H95" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="M95" t="s">
+        <v>174</v>
       </c>
       <c r="P95" t="s">
         <v>175</v>
@@ -6793,40 +6853,37 @@
     </row>
     <row r="96" spans="1:18">
       <c r="A96">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B96" s="4">
-        <v>45476.407210648147</v>
+        <v>45476.448657407411</v>
       </c>
       <c r="C96" s="4">
-        <v>45476.451041666667</v>
+        <v>45476.450624999998</v>
       </c>
       <c r="D96" t="s">
-        <v>160</v>
+        <v>26</v>
       </c>
       <c r="E96" t="s">
-        <v>161</v>
+        <v>27</v>
       </c>
       <c r="F96" t="s">
         <v>20</v>
       </c>
       <c r="G96" s="1">
-        <v>45418</v>
+        <v>45405</v>
       </c>
       <c r="H96" t="s">
-        <v>48</v>
-      </c>
-      <c r="N96">
-        <v>2592</v>
-      </c>
-      <c r="O96">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="P96" t="s">
         <v>176</v>
       </c>
       <c r="Q96" t="s">
-        <v>163</v>
+        <v>30</v>
+      </c>
+      <c r="R96" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="97" spans="1:18">
@@ -11048,25 +11105,25 @@
     </row>
     <row r="204" spans="1:18">
       <c r="A204">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="B204" s="4">
-        <v>45628.442372685196</v>
+        <v>45628.442210648202</v>
       </c>
       <c r="C204" s="4">
-        <v>45628.442673611098</v>
+        <v>45628.491458333301</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E204" s="3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F204" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G204" s="1">
-        <v>45617</v>
+        <v>45519</v>
       </c>
       <c r="H204" s="3" t="s">
         <v>28</v>
@@ -11077,7 +11134,7 @@
         <v>339</v>
       </c>
       <c r="Q204" s="3" t="s">
-        <v>274</v>
+        <v>340</v>
       </c>
       <c r="R204" s="3" t="s">
         <v>193</v>
@@ -11085,53 +11142,50 @@
     </row>
     <row r="205" spans="1:18">
       <c r="A205">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B205" s="4">
-        <v>45628.443796296298</v>
+        <v>45628.442372685196</v>
       </c>
       <c r="C205" s="4">
-        <v>45628.445682870399</v>
+        <v>45628.442673611098</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="E205" s="3" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="F205" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G205" s="1">
-        <v>45496</v>
+        <v>45617</v>
       </c>
       <c r="H205" s="3" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="L205" s="3"/>
       <c r="M205" s="3"/>
-      <c r="O205">
-        <v>5</v>
-      </c>
       <c r="P205" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Q205" s="3" t="s">
-        <v>213</v>
+        <v>274</v>
       </c>
       <c r="R205" s="3" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="206" spans="1:18">
       <c r="A206">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B206" s="4">
-        <v>45628.445729166699</v>
+        <v>45628.443796296298</v>
       </c>
       <c r="C206" s="4">
-        <v>45628.446226851898</v>
+        <v>45628.445682870399</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>58</v>
@@ -11143,30 +11197,35 @@
         <v>20</v>
       </c>
       <c r="G206" s="1">
-        <v>45502</v>
+        <v>45496</v>
       </c>
       <c r="H206" s="3" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="L206" s="3"/>
       <c r="M206" s="3"/>
+      <c r="O206">
+        <v>5</v>
+      </c>
       <c r="P206" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="Q206" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="R206" s="3"/>
+      <c r="R206" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="207" spans="1:18">
       <c r="A207">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B207" s="4">
-        <v>45628.446250000001</v>
+        <v>45628.445729166699</v>
       </c>
       <c r="C207" s="4">
-        <v>45628.449074074102</v>
+        <v>45628.446226851898</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>58</v>
@@ -11178,34 +11237,30 @@
         <v>20</v>
       </c>
       <c r="G207" s="1">
-        <v>45640</v>
+        <v>45502</v>
       </c>
       <c r="H207" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L207" s="3"/>
-      <c r="M207" s="3" t="s">
-        <v>342</v>
-      </c>
+      <c r="M207" s="3"/>
       <c r="P207" s="3" t="s">
         <v>343</v>
       </c>
       <c r="Q207" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="R207" s="3" t="s">
-        <v>186</v>
-      </c>
+      <c r="R207" s="3"/>
     </row>
     <row r="208" spans="1:18">
       <c r="A208">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B208" s="4">
-        <v>45628.449097222197</v>
+        <v>45628.446250000001</v>
       </c>
       <c r="C208" s="4">
-        <v>45628.449675925898</v>
+        <v>45628.449074074102</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>58</v>
@@ -11217,7 +11272,7 @@
         <v>20</v>
       </c>
       <c r="G208" s="1">
-        <v>45565</v>
+        <v>45640</v>
       </c>
       <c r="H208" s="3" t="s">
         <v>21</v>
@@ -11238,13 +11293,13 @@
     </row>
     <row r="209" spans="1:18">
       <c r="A209">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B209" s="4">
-        <v>45628.449687499997</v>
+        <v>45628.449097222197</v>
       </c>
       <c r="C209" s="4">
-        <v>45628.450486111098</v>
+        <v>45628.449675925898</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>58</v>
@@ -11256,18 +11311,17 @@
         <v>20</v>
       </c>
       <c r="G209" s="1">
-        <v>45531</v>
+        <v>45565</v>
       </c>
       <c r="H209" s="3" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="L209" s="3"/>
-      <c r="M209" s="3"/>
-      <c r="O209">
-        <v>6</v>
+      <c r="M209" s="3" t="s">
+        <v>346</v>
       </c>
       <c r="P209" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="Q209" s="3" t="s">
         <v>213</v>
@@ -11278,13 +11332,13 @@
     </row>
     <row r="210" spans="1:18">
       <c r="A210">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B210" s="4">
-        <v>45628.4510069444</v>
+        <v>45628.449687499997</v>
       </c>
       <c r="C210" s="4">
-        <v>45628.451666666697</v>
+        <v>45628.450486111098</v>
       </c>
       <c r="D210" s="3" t="s">
         <v>58</v>
@@ -11296,30 +11350,35 @@
         <v>20</v>
       </c>
       <c r="G210" s="1">
-        <v>45558</v>
+        <v>45531</v>
       </c>
       <c r="H210" s="3" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="L210" s="3"/>
       <c r="M210" s="3"/>
+      <c r="O210">
+        <v>6</v>
+      </c>
       <c r="P210" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="Q210" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="R210" s="3"/>
+      <c r="R210" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="211" spans="1:18">
       <c r="A211">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B211" s="4">
-        <v>45628.4519097222</v>
+        <v>45628.4510069444</v>
       </c>
       <c r="C211" s="4">
-        <v>45628.452094907399</v>
+        <v>45628.451666666697</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>58</v>
@@ -11331,18 +11390,15 @@
         <v>20</v>
       </c>
       <c r="G211" s="1">
-        <v>45552</v>
+        <v>45558</v>
       </c>
       <c r="H211" s="3" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="L211" s="3"/>
       <c r="M211" s="3"/>
-      <c r="O211">
-        <v>4</v>
-      </c>
       <c r="P211" s="3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="Q211" s="3" t="s">
         <v>213</v>
@@ -11351,13 +11407,13 @@
     </row>
     <row r="212" spans="1:18">
       <c r="A212">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B212" s="4">
-        <v>45628.452337962997</v>
+        <v>45628.4519097222</v>
       </c>
       <c r="C212" s="4">
-        <v>45628.452604166698</v>
+        <v>45628.452094907399</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>58</v>
@@ -11369,7 +11425,7 @@
         <v>20</v>
       </c>
       <c r="G212" s="1">
-        <v>45581</v>
+        <v>45552</v>
       </c>
       <c r="H212" s="3" t="s">
         <v>46</v>
@@ -11377,10 +11433,10 @@
       <c r="L212" s="3"/>
       <c r="M212" s="3"/>
       <c r="O212">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P212" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="Q212" s="3" t="s">
         <v>213</v>
@@ -11389,13 +11445,13 @@
     </row>
     <row r="213" spans="1:18">
       <c r="A213">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B213" s="4">
-        <v>45628.452939814801</v>
+        <v>45628.452337962997</v>
       </c>
       <c r="C213" s="4">
-        <v>45628.4531712963</v>
+        <v>45628.452604166698</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>58</v>
@@ -11407,7 +11463,7 @@
         <v>20</v>
       </c>
       <c r="G213" s="1">
-        <v>45610</v>
+        <v>45581</v>
       </c>
       <c r="H213" s="3" t="s">
         <v>46</v>
@@ -11415,10 +11471,10 @@
       <c r="L213" s="3"/>
       <c r="M213" s="3"/>
       <c r="O213">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P213" s="3" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="Q213" s="3" t="s">
         <v>213</v>
@@ -11427,13 +11483,13 @@
     </row>
     <row r="214" spans="1:18">
       <c r="A214">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B214" s="4">
-        <v>45628.453194444402</v>
+        <v>45628.452939814801</v>
       </c>
       <c r="C214" s="4">
-        <v>45628.454583333303</v>
+        <v>45628.4531712963</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>58</v>
@@ -11445,32 +11501,33 @@
         <v>20</v>
       </c>
       <c r="G214" s="1">
-        <v>45544</v>
+        <v>45610</v>
       </c>
       <c r="H214" s="3" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="L214" s="3"/>
       <c r="M214" s="3"/>
+      <c r="O214">
+        <v>2</v>
+      </c>
       <c r="P214" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="Q214" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="R214" s="3" t="s">
-        <v>186</v>
-      </c>
+      <c r="R214" s="3"/>
     </row>
     <row r="215" spans="1:18">
       <c r="A215">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B215" s="4">
-        <v>45628.454594907402</v>
+        <v>45628.453194444402</v>
       </c>
       <c r="C215" s="4">
-        <v>45628.455405092602</v>
+        <v>45628.454583333303</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>58</v>
@@ -11482,7 +11539,7 @@
         <v>20</v>
       </c>
       <c r="G215" s="1">
-        <v>45615</v>
+        <v>45544</v>
       </c>
       <c r="H215" s="3" t="s">
         <v>28</v>
@@ -11490,22 +11547,24 @@
       <c r="L215" s="3"/>
       <c r="M215" s="3"/>
       <c r="P215" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="Q215" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="R215" s="3"/>
+      <c r="R215" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="216" spans="1:18">
       <c r="A216">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B216" s="4">
-        <v>45628.455439814803</v>
+        <v>45628.454594907402</v>
       </c>
       <c r="C216" s="4">
-        <v>45628.455960648098</v>
+        <v>45628.455405092602</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>58</v>
@@ -11517,15 +11576,15 @@
         <v>20</v>
       </c>
       <c r="G216" s="1">
-        <v>45617</v>
+        <v>45615</v>
       </c>
       <c r="H216" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="L216" s="3"/>
       <c r="M216" s="3"/>
       <c r="P216" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="Q216" s="3" t="s">
         <v>213</v>
@@ -11534,13 +11593,13 @@
     </row>
     <row r="217" spans="1:18">
       <c r="A217">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B217" s="4">
-        <v>45628.455972222197</v>
+        <v>45628.455439814803</v>
       </c>
       <c r="C217" s="4">
-        <v>45628.457951388897</v>
+        <v>45628.455960648098</v>
       </c>
       <c r="D217" s="3" t="s">
         <v>58</v>
@@ -11552,15 +11611,13 @@
         <v>20</v>
       </c>
       <c r="G217" s="1">
-        <v>45427</v>
+        <v>45617</v>
       </c>
       <c r="H217" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L217" s="3"/>
-      <c r="M217" s="3" t="s">
-        <v>354</v>
-      </c>
+      <c r="M217" s="3"/>
       <c r="P217" s="3" t="s">
         <v>355</v>
       </c>
@@ -11571,13 +11628,13 @@
     </row>
     <row r="218" spans="1:18">
       <c r="A218">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B218" s="4">
-        <v>45628.458668981497</v>
+        <v>45628.455972222197</v>
       </c>
       <c r="C218" s="4">
-        <v>45628.458969907399</v>
+        <v>45628.457951388897</v>
       </c>
       <c r="D218" s="3" t="s">
         <v>58</v>
@@ -11589,7 +11646,7 @@
         <v>20</v>
       </c>
       <c r="G218" s="1">
-        <v>45580</v>
+        <v>45427</v>
       </c>
       <c r="H218" s="3" t="s">
         <v>21</v>
@@ -11608,13 +11665,13 @@
     </row>
     <row r="219" spans="1:18">
       <c r="A219">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B219" s="4">
-        <v>45628.461122685199</v>
+        <v>45628.458668981497</v>
       </c>
       <c r="C219" s="4">
-        <v>45628.461412037002</v>
+        <v>45628.458969907399</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>58</v>
@@ -11626,7 +11683,7 @@
         <v>20</v>
       </c>
       <c r="G219" s="1">
-        <v>45414</v>
+        <v>45580</v>
       </c>
       <c r="H219" s="3" t="s">
         <v>21</v>
@@ -11641,19 +11698,17 @@
       <c r="Q219" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="R219" s="3" t="s">
-        <v>186</v>
-      </c>
+      <c r="R219" s="3"/>
     </row>
     <row r="220" spans="1:18">
       <c r="A220">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B220" s="4">
-        <v>45628.4614351852</v>
+        <v>45628.461122685199</v>
       </c>
       <c r="C220" s="4">
-        <v>45628.462685185201</v>
+        <v>45628.461412037002</v>
       </c>
       <c r="D220" s="3" t="s">
         <v>58</v>
@@ -11665,7 +11720,7 @@
         <v>20</v>
       </c>
       <c r="G220" s="1">
-        <v>45413</v>
+        <v>45414</v>
       </c>
       <c r="H220" s="3" t="s">
         <v>21</v>
@@ -11680,17 +11735,19 @@
       <c r="Q220" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="R220" s="3"/>
+      <c r="R220" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="221" spans="1:18">
       <c r="A221">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B221" s="4">
-        <v>45628.463032407402</v>
+        <v>45628.4614351852</v>
       </c>
       <c r="C221" s="4">
-        <v>45628.464745370402</v>
+        <v>45628.462685185201</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>58</v>
@@ -11702,7 +11759,7 @@
         <v>20</v>
       </c>
       <c r="G221" s="1">
-        <v>45440</v>
+        <v>45413</v>
       </c>
       <c r="H221" s="3" t="s">
         <v>21</v>
@@ -11717,126 +11774,126 @@
       <c r="Q221" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="R221" s="3" t="s">
-        <v>210</v>
-      </c>
+      <c r="R221" s="3"/>
     </row>
     <row r="222" spans="1:18">
       <c r="A222">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B222" s="4">
-        <v>45628.467418981498</v>
+        <v>45628.463032407402</v>
       </c>
       <c r="C222" s="4">
-        <v>45628.469340277799</v>
+        <v>45628.464745370402</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>141</v>
+        <v>58</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>142</v>
+        <v>59</v>
       </c>
       <c r="F222" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G222" s="1">
-        <v>45624</v>
+        <v>45440</v>
       </c>
       <c r="H222" s="3" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="L222" s="3"/>
-      <c r="M222" s="3"/>
-      <c r="N222">
-        <v>60</v>
-      </c>
-      <c r="O222">
-        <v>20</v>
+      <c r="M222" s="3" t="s">
+        <v>364</v>
       </c>
       <c r="P222" s="3" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="Q222" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="R222" s="3"/>
+        <v>213</v>
+      </c>
+      <c r="R222" s="3" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="223" spans="1:18">
       <c r="A223">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B223" s="4">
-        <v>45628.482939814799</v>
+        <v>45628.467418981498</v>
       </c>
       <c r="C223" s="4">
-        <v>45628.4841087963</v>
+        <v>45628.469340277799</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>187</v>
+        <v>141</v>
       </c>
       <c r="E223" s="3" t="s">
-        <v>188</v>
+        <v>142</v>
       </c>
       <c r="F223" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G223" s="1">
-        <v>45628</v>
+        <v>45624</v>
       </c>
       <c r="H223" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L223" s="3"/>
       <c r="M223" s="3"/>
+      <c r="N223">
+        <v>60</v>
+      </c>
       <c r="O223">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="P223" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="Q223" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="R223" s="3" t="s">
-        <v>186</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="R223" s="3"/>
     </row>
     <row r="224" spans="1:18">
       <c r="A224">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B224" s="4">
-        <v>45628.442210648202</v>
+        <v>45628.482939814799</v>
       </c>
       <c r="C224" s="4">
-        <v>45628.491458333301</v>
+        <v>45628.4841087963</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>27</v>
+        <v>188</v>
       </c>
       <c r="F224" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G224" s="1">
-        <v>45519</v>
+        <v>45628</v>
       </c>
       <c r="H224" s="3" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="L224" s="3"/>
       <c r="M224" s="3"/>
+      <c r="O224">
+        <v>6</v>
+      </c>
       <c r="P224" s="3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="Q224" s="3" t="s">
-        <v>367</v>
+        <v>190</v>
       </c>
       <c r="R224" s="3" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="225" spans="1:18">
@@ -11873,7 +11930,7 @@
         <v>368</v>
       </c>
       <c r="Q225" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R225" s="3" t="s">
         <v>193</v>
@@ -11916,7 +11973,7 @@
         <v>369</v>
       </c>
       <c r="Q226" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R226" s="3" t="s">
         <v>193</v>
@@ -12076,7 +12133,7 @@
         <v>375</v>
       </c>
       <c r="Q230" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R230" s="3" t="s">
         <v>193</v>
@@ -12116,7 +12173,7 @@
         <v>376</v>
       </c>
       <c r="Q231" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R231" s="3" t="s">
         <v>193</v>
@@ -12156,7 +12213,7 @@
         <v>377</v>
       </c>
       <c r="Q232" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R232" s="3" t="s">
         <v>193</v>
@@ -12193,7 +12250,7 @@
         <v>378</v>
       </c>
       <c r="Q233" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R233" s="3" t="s">
         <v>193</v>
@@ -12236,7 +12293,7 @@
         <v>379</v>
       </c>
       <c r="Q234" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R234" s="3" t="s">
         <v>193</v>
@@ -12275,7 +12332,7 @@
       </c>
       <c r="P235" s="3"/>
       <c r="Q235" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R235" s="3" t="s">
         <v>275</v>
@@ -12355,7 +12412,7 @@
         <v>386</v>
       </c>
       <c r="Q237" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R237" s="3" t="s">
         <v>275</v>
@@ -12664,79 +12721,79 @@
     </row>
     <row r="246" spans="1:18">
       <c r="A246">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B246" s="4">
-        <v>45629.471516203703</v>
+        <v>45629.471006944397</v>
       </c>
       <c r="C246" s="4">
-        <v>45629.472511574102</v>
+        <v>45629.473240740699</v>
       </c>
       <c r="D246" s="3" t="s">
-        <v>160</v>
+        <v>187</v>
       </c>
       <c r="E246" s="3" t="s">
-        <v>161</v>
+        <v>188</v>
       </c>
       <c r="F246" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G246" s="1">
-        <v>45529</v>
+        <v>45574</v>
       </c>
       <c r="H246" s="3" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="L246" s="3"/>
       <c r="M246" s="3"/>
-      <c r="O246">
-        <v>10</v>
-      </c>
       <c r="P246" s="3" t="s">
         <v>399</v>
       </c>
       <c r="Q246" s="3" t="s">
-        <v>274</v>
+        <v>190</v>
       </c>
       <c r="R246" s="3" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="247" spans="1:18">
       <c r="A247">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B247" s="4">
-        <v>45629.471006944397</v>
+        <v>45629.471516203703</v>
       </c>
       <c r="C247" s="4">
-        <v>45629.473240740699</v>
+        <v>45629.472511574102</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="E247" s="3" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="F247" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G247" s="1">
-        <v>45574</v>
+        <v>45529</v>
       </c>
       <c r="H247" s="3" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="L247" s="3"/>
       <c r="M247" s="3"/>
+      <c r="O247">
+        <v>10</v>
+      </c>
       <c r="P247" s="3" t="s">
         <v>400</v>
       </c>
       <c r="Q247" s="3" t="s">
-        <v>190</v>
+        <v>274</v>
       </c>
       <c r="R247" s="3" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="248" spans="1:18">
@@ -12857,81 +12914,81 @@
     </row>
     <row r="251" spans="1:18">
       <c r="A251">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B251" s="4">
-        <v>45629.4750347222</v>
+        <v>45629.474513888897</v>
       </c>
       <c r="C251" s="4">
-        <v>45629.477905092601</v>
+        <v>45629.479039351798</v>
       </c>
       <c r="D251" s="3" t="s">
-        <v>90</v>
+        <v>187</v>
       </c>
       <c r="E251" s="3" t="s">
-        <v>91</v>
+        <v>188</v>
       </c>
       <c r="F251" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G251" s="1">
-        <v>45481</v>
+        <v>45607</v>
       </c>
       <c r="H251" s="3" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="L251" s="3"/>
       <c r="M251" s="3"/>
+      <c r="N251">
+        <v>440</v>
+      </c>
+      <c r="O251">
+        <v>0</v>
+      </c>
       <c r="P251" s="3" t="s">
         <v>405</v>
       </c>
       <c r="Q251" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="R251" s="3"/>
+        <v>190</v>
+      </c>
+      <c r="R251" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="252" spans="1:18">
       <c r="A252">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B252" s="4">
-        <v>45629.474513888897</v>
+        <v>45629.4750347222</v>
       </c>
       <c r="C252" s="4">
-        <v>45629.479039351798</v>
+        <v>45629.477905092601</v>
       </c>
       <c r="D252" s="3" t="s">
-        <v>187</v>
+        <v>90</v>
       </c>
       <c r="E252" s="3" t="s">
-        <v>188</v>
+        <v>91</v>
       </c>
       <c r="F252" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G252" s="1">
-        <v>45607</v>
+        <v>45481</v>
       </c>
       <c r="H252" s="3" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="L252" s="3"/>
       <c r="M252" s="3"/>
-      <c r="N252">
-        <v>440</v>
-      </c>
-      <c r="O252">
-        <v>0</v>
-      </c>
       <c r="P252" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="Q252" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="Q252" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="R252" s="3" t="s">
-        <v>186</v>
-      </c>
+      <c r="R252" s="3"/>
     </row>
     <row r="253" spans="1:18">
       <c r="A253">
@@ -12976,50 +13033,53 @@
     </row>
     <row r="254" spans="1:18">
       <c r="A254">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B254" s="4">
-        <v>45629.479085648098</v>
+        <v>45629.478055555599</v>
       </c>
       <c r="C254" s="4">
-        <v>45629.480173611097</v>
+        <v>45629.482025463003</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="E254" s="3" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="F254" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G254" s="1">
-        <v>45421</v>
+        <v>45502</v>
       </c>
       <c r="H254" s="3" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="L254" s="3"/>
       <c r="M254" s="3"/>
+      <c r="O254">
+        <v>4</v>
+      </c>
       <c r="P254" s="3" t="s">
         <v>409</v>
       </c>
       <c r="Q254" s="3" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="R254" s="3" t="s">
-        <v>410</v>
+        <v>186</v>
       </c>
     </row>
     <row r="255" spans="1:18">
       <c r="A255">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B255" s="4">
-        <v>45629.480833333299</v>
+        <v>45629.479085648098</v>
       </c>
       <c r="C255" s="4">
-        <v>45629.481215277803</v>
+        <v>45629.480173611097</v>
       </c>
       <c r="D255" s="3" t="s">
         <v>114</v>
@@ -13031,7 +13091,7 @@
         <v>20</v>
       </c>
       <c r="G255" s="1">
-        <v>45374</v>
+        <v>45421</v>
       </c>
       <c r="H255" s="3" t="s">
         <v>28</v>
@@ -13039,13 +13099,13 @@
       <c r="L255" s="3"/>
       <c r="M255" s="3"/>
       <c r="P255" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="Q255" s="3" t="s">
         <v>209</v>
       </c>
       <c r="R255" s="3" t="s">
-        <v>247</v>
+        <v>411</v>
       </c>
     </row>
     <row r="256" spans="1:18">
@@ -13087,42 +13147,39 @@
     </row>
     <row r="257" spans="1:18">
       <c r="A257">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B257" s="4">
-        <v>45629.478055555599</v>
+        <v>45629.480833333299</v>
       </c>
       <c r="C257" s="4">
-        <v>45629.482025463003</v>
+        <v>45629.481215277803</v>
       </c>
       <c r="D257" s="3" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="E257" s="3" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="F257" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G257" s="1">
-        <v>45502</v>
+        <v>45374</v>
       </c>
       <c r="H257" s="3" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="L257" s="3"/>
       <c r="M257" s="3"/>
-      <c r="O257">
-        <v>4</v>
-      </c>
       <c r="P257" s="3" t="s">
         <v>413</v>
       </c>
       <c r="Q257" s="3" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="R257" s="3" t="s">
-        <v>186</v>
+        <v>247</v>
       </c>
     </row>
     <row r="258" spans="1:18">
@@ -13761,25 +13818,25 @@
     </row>
     <row r="274" spans="1:18">
       <c r="A274">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B274" s="4">
-        <v>45629.499826388899</v>
+        <v>45629.499131944402</v>
       </c>
       <c r="C274" s="4">
-        <v>45629.500891203701</v>
+        <v>45629.554537037002</v>
       </c>
       <c r="D274" s="3" t="s">
-        <v>229</v>
+        <v>160</v>
       </c>
       <c r="E274" s="3" t="s">
-        <v>230</v>
+        <v>161</v>
       </c>
       <c r="F274" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G274" s="1">
-        <v>45580</v>
+        <v>45609</v>
       </c>
       <c r="H274" s="3" t="s">
         <v>48</v>
@@ -13787,30 +13844,28 @@
       <c r="L274" s="3"/>
       <c r="M274" s="3"/>
       <c r="N274">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="O274">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="P274" s="3" t="s">
         <v>430</v>
       </c>
       <c r="Q274" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="R274" s="3" t="s">
-        <v>236</v>
-      </c>
+        <v>393</v>
+      </c>
+      <c r="R274" s="3"/>
     </row>
     <row r="275" spans="1:18">
       <c r="A275">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B275" s="4">
-        <v>45629.5009027778</v>
+        <v>45629.499826388899</v>
       </c>
       <c r="C275" s="4">
-        <v>45629.501828703702</v>
+        <v>45629.500891203701</v>
       </c>
       <c r="D275" s="3" t="s">
         <v>229</v>
@@ -13822,13 +13877,16 @@
         <v>20</v>
       </c>
       <c r="G275" s="1">
-        <v>45566</v>
+        <v>45580</v>
       </c>
       <c r="H275" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L275" s="3"/>
       <c r="M275" s="3"/>
+      <c r="N275">
+        <v>2</v>
+      </c>
       <c r="O275">
         <v>6</v>
       </c>
@@ -13844,13 +13902,13 @@
     </row>
     <row r="276" spans="1:18">
       <c r="A276">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B276" s="4">
-        <v>45629.501851851797</v>
+        <v>45629.5009027778</v>
       </c>
       <c r="C276" s="4">
-        <v>45629.503020833297</v>
+        <v>45629.501828703702</v>
       </c>
       <c r="D276" s="3" t="s">
         <v>229</v>
@@ -13862,7 +13920,7 @@
         <v>20</v>
       </c>
       <c r="G276" s="1">
-        <v>45543</v>
+        <v>45566</v>
       </c>
       <c r="H276" s="3" t="s">
         <v>46</v>
@@ -13876,7 +13934,7 @@
         <v>432</v>
       </c>
       <c r="Q276" s="3" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="R276" s="3" t="s">
         <v>236</v>
@@ -13884,44 +13942,43 @@
     </row>
     <row r="277" spans="1:18">
       <c r="A277">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B277" s="4">
-        <v>45629.499131944402</v>
+        <v>45629.501851851797</v>
       </c>
       <c r="C277" s="4">
-        <v>45629.554537037002</v>
+        <v>45629.503020833297</v>
       </c>
       <c r="D277" s="3" t="s">
-        <v>160</v>
+        <v>229</v>
       </c>
       <c r="E277" s="3" t="s">
-        <v>161</v>
+        <v>230</v>
       </c>
       <c r="F277" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G277" s="1">
-        <v>45609</v>
+        <v>45543</v>
       </c>
       <c r="H277" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L277" s="3"/>
       <c r="M277" s="3"/>
-      <c r="N277">
-        <v>10</v>
-      </c>
       <c r="O277">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="P277" s="3" t="s">
         <v>433</v>
       </c>
       <c r="Q277" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="R277" s="3"/>
+        <v>232</v>
+      </c>
+      <c r="R277" s="3" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="278" spans="1:18">
       <c r="A278">
@@ -14565,84 +14622,84 @@
     </row>
     <row r="294" spans="1:18">
       <c r="A294">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B294" s="4">
-        <v>45629.642939814803</v>
+        <v>45629.6427430556</v>
       </c>
       <c r="C294" s="4">
-        <v>45629.644004629597</v>
+        <v>45629.644317129598</v>
       </c>
       <c r="D294" s="3" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="E294" s="3" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="F294" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G294" s="1">
-        <v>45657</v>
+        <v>44436</v>
       </c>
       <c r="H294" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L294" s="3"/>
-      <c r="M294" s="3"/>
-      <c r="N294">
-        <v>30</v>
-      </c>
-      <c r="O294">
-        <v>2</v>
-      </c>
-      <c r="P294" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L294" s="3" t="s">
         <v>452</v>
       </c>
+      <c r="M294" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="P294" s="3"/>
       <c r="Q294" s="3" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="R294" s="3" t="s">
-        <v>186</v>
+        <v>236</v>
       </c>
     </row>
     <row r="295" spans="1:18">
       <c r="A295">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B295" s="4">
-        <v>45629.6427430556</v>
+        <v>45629.642939814803</v>
       </c>
       <c r="C295" s="4">
-        <v>45629.644317129598</v>
+        <v>45629.644004629597</v>
       </c>
       <c r="D295" s="3" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="E295" s="3" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="F295" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G295" s="1">
-        <v>44436</v>
+        <v>45657</v>
       </c>
       <c r="H295" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L295" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="M295" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L295" s="3"/>
+      <c r="M295" s="3"/>
+      <c r="N295">
+        <v>30</v>
+      </c>
+      <c r="O295">
+        <v>2</v>
+      </c>
+      <c r="P295" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="P295" s="3"/>
       <c r="Q295" s="3" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="R295" s="3" t="s">
-        <v>236</v>
+        <v>186</v>
       </c>
     </row>
     <row r="296" spans="1:18">
@@ -16364,7 +16421,7 @@
         <v>521</v>
       </c>
       <c r="Q341" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R341" s="3" t="s">
         <v>193</v>
@@ -16407,7 +16464,7 @@
         <v>522</v>
       </c>
       <c r="Q342" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R342" s="3" t="s">
         <v>193</v>
@@ -16444,7 +16501,7 @@
         <v>523</v>
       </c>
       <c r="Q343" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R343" s="3" t="s">
         <v>193</v>
@@ -16688,7 +16745,7 @@
         <v>530</v>
       </c>
       <c r="Q349" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R349" s="3" t="s">
         <v>191</v>
@@ -17812,7 +17869,7 @@
         <v>571</v>
       </c>
       <c r="Q378" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R378" s="3" t="s">
         <v>275</v>
@@ -17849,7 +17906,7 @@
         <v>572</v>
       </c>
       <c r="Q379" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R379" s="3" t="s">
         <v>193</v>
@@ -18732,7 +18789,7 @@
       </c>
       <c r="P402" s="3"/>
       <c r="Q402" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R402" s="3" t="s">
         <v>275</v>
@@ -18771,7 +18828,7 @@
       </c>
       <c r="P403" s="3"/>
       <c r="Q403" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R403" s="3" t="s">
         <v>275</v>
@@ -18814,7 +18871,7 @@
         <v>609</v>
       </c>
       <c r="Q404" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R404" s="3" t="s">
         <v>193</v>
@@ -18857,7 +18914,7 @@
         <v>610</v>
       </c>
       <c r="Q405" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R405" s="3" t="s">
         <v>193</v>
@@ -18900,7 +18957,7 @@
         <v>611</v>
       </c>
       <c r="Q406" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R406" s="3" t="s">
         <v>193</v>
@@ -18937,7 +18994,7 @@
         <v>612</v>
       </c>
       <c r="Q407" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R407" s="3" t="s">
         <v>193</v>
@@ -18980,7 +19037,7 @@
         <v>613</v>
       </c>
       <c r="Q408" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R408" s="3" t="s">
         <v>275</v>
@@ -19023,7 +19080,7 @@
         <v>614</v>
       </c>
       <c r="Q409" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R409" s="3" t="s">
         <v>193</v>
@@ -19066,7 +19123,7 @@
         <v>615</v>
       </c>
       <c r="Q410" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R410" s="3" t="s">
         <v>193</v>
@@ -20252,7 +20309,7 @@
         <v>652</v>
       </c>
       <c r="Q440" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R440" s="3" t="s">
         <v>193</v>
@@ -20603,7 +20660,7 @@
       </c>
       <c r="P449" s="3"/>
       <c r="Q449" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R449" s="3" t="s">
         <v>275</v>
@@ -20642,7 +20699,7 @@
       </c>
       <c r="P450" s="3"/>
       <c r="Q450" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R450" s="3" t="s">
         <v>193</v>
@@ -20681,7 +20738,7 @@
       </c>
       <c r="P451" s="3"/>
       <c r="Q451" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R451" s="3" t="s">
         <v>193</v>
@@ -21841,7 +21898,7 @@
         <v>725</v>
       </c>
       <c r="Q481" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R481" s="3" t="s">
         <v>193</v>
@@ -24413,7 +24470,7 @@
         <v>814</v>
       </c>
       <c r="Q547" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R547" s="3" t="s">
         <v>193</v>
@@ -24450,7 +24507,7 @@
         <v>815</v>
       </c>
       <c r="Q548" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R548" s="3" t="s">
         <v>193</v>
@@ -24487,7 +24544,7 @@
         <v>816</v>
       </c>
       <c r="Q549" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R549" s="3" t="s">
         <v>193</v>
@@ -24524,7 +24581,7 @@
         <v>817</v>
       </c>
       <c r="Q550" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R550" s="3" t="s">
         <v>193</v>
@@ -24561,7 +24618,7 @@
         <v>818</v>
       </c>
       <c r="Q551" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R551" s="3" t="s">
         <v>193</v>
@@ -24598,7 +24655,7 @@
         <v>819</v>
       </c>
       <c r="Q552" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R552" s="3" t="s">
         <v>275</v>
@@ -24635,7 +24692,7 @@
         <v>820</v>
       </c>
       <c r="Q553" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R553" s="3" t="s">
         <v>275</v>
@@ -24672,7 +24729,7 @@
         <v>821</v>
       </c>
       <c r="Q554" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R554" s="3" t="s">
         <v>275</v>
@@ -24709,7 +24766,7 @@
         <v>822</v>
       </c>
       <c r="Q555" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R555" s="3" t="s">
         <v>275</v>
@@ -24783,7 +24840,7 @@
         <v>825</v>
       </c>
       <c r="Q557" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R557" s="3" t="s">
         <v>193</v>
@@ -24820,7 +24877,7 @@
         <v>826</v>
       </c>
       <c r="Q558" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R558" s="3" t="s">
         <v>275</v>
@@ -24857,7 +24914,7 @@
         <v>827</v>
       </c>
       <c r="Q559" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R559" s="3" t="s">
         <v>275</v>
@@ -25494,7 +25551,7 @@
       </c>
       <c r="P576" s="3"/>
       <c r="Q576" s="3" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="R576" s="3" t="s">
         <v>275</v>
@@ -26537,6 +26594,389 @@
       <c r="R603" s="3" t="s">
         <v>236</v>
       </c>
+    </row>
+    <row r="604" spans="1:18">
+      <c r="A604">
+        <v>605</v>
+      </c>
+      <c r="B604" s="4">
+        <v>46058.612083333297</v>
+      </c>
+      <c r="C604" s="4">
+        <v>46058.612662036998</v>
+      </c>
+      <c r="D604" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="E604" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="F604" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G604" s="1">
+        <v>46034</v>
+      </c>
+      <c r="H604" s="3" t="s">
+        <v>887</v>
+      </c>
+      <c r="L604" s="3"/>
+      <c r="M604" s="3"/>
+      <c r="O604">
+        <v>14</v>
+      </c>
+      <c r="P604" s="3" t="s">
+        <v>888</v>
+      </c>
+      <c r="Q604" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="R604" s="3"/>
+    </row>
+    <row r="605" spans="1:18">
+      <c r="A605">
+        <v>606</v>
+      </c>
+      <c r="B605" s="4">
+        <v>46058.618865740696</v>
+      </c>
+      <c r="C605" s="4">
+        <v>46058.620451388902</v>
+      </c>
+      <c r="D605" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E605" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F605" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G605" s="1">
+        <v>46043</v>
+      </c>
+      <c r="H605" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="J605" t="s">
+        <v>890</v>
+      </c>
+      <c r="L605" s="3"/>
+      <c r="M605" s="3"/>
+      <c r="P605" s="3" t="s">
+        <v>891</v>
+      </c>
+      <c r="Q605" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="R605" s="3"/>
+    </row>
+    <row r="606" spans="1:18">
+      <c r="A606">
+        <v>607</v>
+      </c>
+      <c r="B606" s="4">
+        <v>46058.620567129597</v>
+      </c>
+      <c r="C606" s="4">
+        <v>46058.621168981503</v>
+      </c>
+      <c r="D606" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E606" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F606" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G606" s="1">
+        <v>46049</v>
+      </c>
+      <c r="H606" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="J606" t="s">
+        <v>892</v>
+      </c>
+      <c r="L606" s="3"/>
+      <c r="M606" s="3"/>
+      <c r="P606" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="Q606" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="R606" s="3"/>
+    </row>
+    <row r="607" spans="1:18">
+      <c r="A607">
+        <v>608</v>
+      </c>
+      <c r="B607" s="4">
+        <v>46058.621192129598</v>
+      </c>
+      <c r="C607" s="4">
+        <v>46058.621759259302</v>
+      </c>
+      <c r="D607" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E607" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F607" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G607" s="1">
+        <v>46049</v>
+      </c>
+      <c r="H607" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="J607" t="s">
+        <v>892</v>
+      </c>
+      <c r="L607" s="3"/>
+      <c r="M607" s="3"/>
+      <c r="P607" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="Q607" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="R607" s="3"/>
+    </row>
+    <row r="608" spans="1:18">
+      <c r="A608">
+        <v>609</v>
+      </c>
+      <c r="B608" s="4">
+        <v>46058.621967592597</v>
+      </c>
+      <c r="C608" s="4">
+        <v>46058.623865740701</v>
+      </c>
+      <c r="D608" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E608" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F608" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G608" s="1">
+        <v>46056</v>
+      </c>
+      <c r="H608" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="I608" t="s">
+        <v>896</v>
+      </c>
+      <c r="L608" s="3"/>
+      <c r="M608" s="3"/>
+      <c r="P608" s="3" t="s">
+        <v>897</v>
+      </c>
+      <c r="Q608" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="R608" s="3"/>
+    </row>
+    <row r="609" spans="1:18">
+      <c r="A609">
+        <v>610</v>
+      </c>
+      <c r="B609" s="4">
+        <v>46058.623912037001</v>
+      </c>
+      <c r="C609" s="4">
+        <v>46058.624780092599</v>
+      </c>
+      <c r="D609" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E609" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F609" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G609" s="1">
+        <v>46051</v>
+      </c>
+      <c r="H609" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="K609" t="s">
+        <v>899</v>
+      </c>
+      <c r="L609" s="3"/>
+      <c r="M609" s="3"/>
+      <c r="O609">
+        <v>1</v>
+      </c>
+      <c r="P609" s="3" t="s">
+        <v>900</v>
+      </c>
+      <c r="Q609" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="R609" s="3"/>
+    </row>
+    <row r="610" spans="1:18">
+      <c r="A610">
+        <v>611</v>
+      </c>
+      <c r="B610" s="4">
+        <v>46059.417604166701</v>
+      </c>
+      <c r="C610" s="4">
+        <v>46059.419004629599</v>
+      </c>
+      <c r="D610" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E610" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F610" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G610" s="1">
+        <v>46057</v>
+      </c>
+      <c r="H610" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="I610" t="s">
+        <v>896</v>
+      </c>
+      <c r="L610" s="3"/>
+      <c r="M610" s="3"/>
+      <c r="P610" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="Q610" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="R610" s="3"/>
+    </row>
+    <row r="611" spans="1:18">
+      <c r="A611">
+        <v>612</v>
+      </c>
+      <c r="B611" s="4">
+        <v>46059.419050925899</v>
+      </c>
+      <c r="C611" s="4">
+        <v>46059.420648148203</v>
+      </c>
+      <c r="D611" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E611" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F611" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G611" s="1">
+        <v>46036</v>
+      </c>
+      <c r="H611" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="J611" t="s">
+        <v>892</v>
+      </c>
+      <c r="L611" s="3"/>
+      <c r="M611" s="3"/>
+      <c r="P611" s="3" t="s">
+        <v>902</v>
+      </c>
+      <c r="Q611" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="R611" s="3"/>
+    </row>
+    <row r="612" spans="1:18">
+      <c r="A612">
+        <v>613</v>
+      </c>
+      <c r="B612" s="4">
+        <v>46059.421458333301</v>
+      </c>
+      <c r="C612" s="4">
+        <v>46059.422025462998</v>
+      </c>
+      <c r="D612" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E612" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F612" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G612" s="1">
+        <v>45995</v>
+      </c>
+      <c r="H612" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="J612" t="s">
+        <v>892</v>
+      </c>
+      <c r="L612" s="3"/>
+      <c r="M612" s="3"/>
+      <c r="P612" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="Q612" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="R612" s="3"/>
+    </row>
+    <row r="613" spans="1:18">
+      <c r="A613">
+        <v>614</v>
+      </c>
+      <c r="B613" s="4">
+        <v>46059.422048611101</v>
+      </c>
+      <c r="C613" s="4">
+        <v>46059.424201388902</v>
+      </c>
+      <c r="D613" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E613" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F613" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G613" s="1">
+        <v>45974</v>
+      </c>
+      <c r="H613" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="J613" t="s">
+        <v>892</v>
+      </c>
+      <c r="L613" s="3"/>
+      <c r="M613" s="3"/>
+      <c r="P613" s="3" t="s">
+        <v>904</v>
+      </c>
+      <c r="Q613" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="R613" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>